<commit_message>
scaling weather amount with volume. still need to erraticism, then tooltips, then (maybe) clouds
</commit_message>
<xml_diff>
--- a/Documents/TestingTable.xlsx
+++ b/Documents/TestingTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b013728n\Documents\GitHub\ToolsDevForEngines\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B0437A2-F9EC-4ADA-A082-30F617C42E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC9A661-3160-4E05-845F-8AB2FC209E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CFA27033-66C9-4DCC-86CD-736E875A59B1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CFA27033-66C9-4DCC-86CD-736E875A59B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
   <si>
     <t>Test Number</t>
   </si>
@@ -159,6 +159,30 @@
   </si>
   <si>
     <t>Adjust bool checks</t>
+  </si>
+  <si>
+    <t>Snow and rain do not spawn simultaneously</t>
+  </si>
+  <si>
+    <t>Scale weather amount with volume size</t>
+  </si>
+  <si>
+    <t>Rain spawn rate should be higher for large volume and lower for small</t>
+  </si>
+  <si>
+    <t>Particle count maxed out</t>
+  </si>
+  <si>
+    <t>Adjust scaling calculation</t>
+  </si>
+  <si>
+    <t>Not enough particles spawning</t>
+  </si>
+  <si>
+    <t>Working, but more adjustment needed. Needs to scale better with very large volumes</t>
+  </si>
+  <si>
+    <t>Adjust scaling calculation with cube root</t>
   </si>
 </sst>
 </file>
@@ -168,7 +192,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,8 +352,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,25 +377,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -451,95 +478,58 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
+      <font>
+        <i val="0"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
+      <font>
+        <i val="0"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-      <border>
+      <font>
+        <i val="0"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -565,6 +555,20 @@
       <font>
         <i val="0"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -577,8 +581,12 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -595,9 +603,7 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -614,7 +620,28 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -628,169 +655,8 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+        <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
   </dxfs>
@@ -813,17 +679,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB7C8FB5-4A60-4589-8AF2-3974B4223A79}" name="Table2" displayName="Table2" ref="A2:H12" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowBorderDxfId="21" tableBorderDxfId="22">
-  <autoFilter ref="A2:H12" xr:uid="{FB7C8FB5-4A60-4589-8AF2-3974B4223A79}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB7C8FB5-4A60-4589-8AF2-3974B4223A79}" name="Table2" displayName="Table2" ref="A2:H19" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+  <autoFilter ref="A2:H19" xr:uid="{FB7C8FB5-4A60-4589-8AF2-3974B4223A79}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D94DCF1D-6FD5-453C-A46D-9869C38352C8}" name="Test Number" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{A020788D-1D41-4852-9F55-934D91AFA649}" name="Climate + Season" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{6185D29F-D1FE-4971-966C-56AC01B5DC76}" name="Test" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{CC5DF699-CAB0-42B7-9B93-2010CA39B689}" name="Expected Behaviour" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{2376F1A1-CD88-4A07-B52B-FC693313EC8D}" name="Actual Behaviour" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{BD349D04-C2F0-46B6-B369-DBCD3900AEDA}" name="Time" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{8DAE1A83-CC84-487F-BD95-98F6B547DCD1}" name="Success?" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{8BF98F09-E2CC-4F11-8A7A-A33C92D265B4}" name="Fix" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{D94DCF1D-6FD5-453C-A46D-9869C38352C8}" name="Test Number" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{A020788D-1D41-4852-9F55-934D91AFA649}" name="Climate + Season" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{6185D29F-D1FE-4971-966C-56AC01B5DC76}" name="Test" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{CC5DF699-CAB0-42B7-9B93-2010CA39B689}" name="Expected Behaviour" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{2376F1A1-CD88-4A07-B52B-FC693313EC8D}" name="Actual Behaviour" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{BD349D04-C2F0-46B6-B369-DBCD3900AEDA}" name="Time" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{8DAE1A83-CC84-487F-BD95-98F6B547DCD1}" name="Success?" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{8BF98F09-E2CC-4F11-8A7A-A33C92D265B4}" name="Fix" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1146,306 +1012,469 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4EA2CC5-2E47-478A-8876-EC323C3D42FE}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="94.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="76.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="9">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="8">
         <v>45702.570138888892</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="12">
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="10">
         <v>45702.578472222223</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="12">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="10">
         <v>45702.595138888886</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="9">
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="10">
         <v>45702.598611111112</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="12">
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="10">
         <v>45702.606944444444</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="12">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="10">
         <v>45702.607638888891</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12" t="s">
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="10">
         <v>45702.619444444441</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="10">
         <v>45702.626388888886</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12" t="s">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="10">
         <v>45702.629166666666</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="10">
         <v>45702.632638888892</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="6" t="s">
         <v>40</v>
       </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="18">
+        <v>45702.720138888886</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="18">
+        <v>45702.743055555555</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="18">
+        <v>45702.744444444441</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="18">
+        <v>45702.745833333334</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="18">
+        <v>45702.75</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="18">
+        <v>45703.786805555559</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G3:G357">
+  <conditionalFormatting sqref="G3:G362">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Indeterminate">
       <formula>NOT(ISERROR(SEARCH("Indeterminate",G3)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
fixed weather transitions and weather scaling, and implemented erraticism. need to finish setup fro snow and wind, then write tooltips, then end. maybe try clouds on tuesday but it doesn't matter for handin if it doesn't work. also kept up with testing doc
</commit_message>
<xml_diff>
--- a/Documents/TestingTable.xlsx
+++ b/Documents/TestingTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b013728n\Documents\GitHub\ToolsDevForEngines\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC9A661-3160-4E05-845F-8AB2FC209E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2729F559-748E-4149-9060-EF9D44E0187A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CFA27033-66C9-4DCC-86CD-736E875A59B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="86">
   <si>
     <t>Test Number</t>
   </si>
@@ -86,9 +86,6 @@
     <t>In weather types with both snow and rain possible, the two should not occur simultaneously</t>
   </si>
   <si>
-    <t>No weather spawning, fix in code with new conditions based on its data table information</t>
-  </si>
-  <si>
     <t>Low rain should be affected by low wind</t>
   </si>
   <si>
@@ -183,6 +180,120 @@
   </si>
   <si>
     <t>Adjust scaling calculation with cube root</t>
+  </si>
+  <si>
+    <t>Softening of transitions between weather states</t>
+  </si>
+  <si>
+    <t>Transitions more softly, but now it will never reach zero</t>
+  </si>
+  <si>
+    <t>Rain should become closer to the next value before actually transitioning</t>
+  </si>
+  <si>
+    <t>Debug while loop; it isn't actually looping</t>
+  </si>
+  <si>
+    <t>Try using tick</t>
+  </si>
+  <si>
+    <t>Make function for calling timer</t>
+  </si>
+  <si>
+    <t>Transitions more softly and can still reach zero</t>
+  </si>
+  <si>
+    <t>Erraticism factor should affect rate of transition</t>
+  </si>
+  <si>
+    <t>Higher erraticism values should have faster transitions, lower should have slower</t>
+  </si>
+  <si>
+    <t>Transitioning too fast for both high values and low values</t>
+  </si>
+  <si>
+    <t>Wasn't setting erraticism in struct from user input</t>
+  </si>
+  <si>
+    <t>Lower values are transitioning faster, higher are slower</t>
+  </si>
+  <si>
+    <t>Change timer calculations</t>
+  </si>
+  <si>
+    <t>High values have fast transitions and low have slow, but softening time is too long</t>
+  </si>
+  <si>
+    <t>Inverse of softening rate is being applied</t>
+  </si>
+  <si>
+    <t>Softening time should be proportional to erraticism factor</t>
+  </si>
+  <si>
+    <t>Softening is being called too soon because it is within the transition timer</t>
+  </si>
+  <si>
+    <t>Create a timer manager</t>
+  </si>
+  <si>
+    <t>Program failed to build because of recursion causing stack overflow</t>
+  </si>
+  <si>
+    <t>Create a softening manager</t>
+  </si>
+  <si>
+    <t>Create a delay</t>
+  </si>
+  <si>
+    <t>Transitions, but correct softening is inconsistent</t>
+  </si>
+  <si>
+    <t>Soften calculation is getting incorrect elements from queue</t>
+  </si>
+  <si>
+    <t>Incrementing head of queue</t>
+  </si>
+  <si>
+    <t>Spawn rate should soften to midpoint of current and next weather</t>
+  </si>
+  <si>
+    <t>Softening to midpoint with rate proportional to erraticism</t>
+  </si>
+  <si>
+    <t>Mediterranean, Winter</t>
+  </si>
+  <si>
+    <t>Low rain</t>
+  </si>
+  <si>
+    <t>Extremely high rain</t>
+  </si>
+  <si>
+    <t>Weather is scaling inversely</t>
+  </si>
+  <si>
+    <t>Climate|Seasons with low rain should have low rain, and high should have high, rather than doing the opposite and scaling inversely</t>
+  </si>
+  <si>
+    <t>Low rain Climate|Season has low rain, high rain has high rain</t>
+  </si>
+  <si>
+    <t>Should have high rainfall no matter the size of the volume</t>
+  </si>
+  <si>
+    <t>High rainfall no matter the size of the volume</t>
+  </si>
+  <si>
+    <t>Should have low rainfall no matter the size of the volume</t>
+  </si>
+  <si>
+    <t>Low rainfall no matter the size of the volume</t>
+  </si>
+  <si>
+    <t>Weather spawning</t>
+  </si>
+  <si>
+    <t>Fix in code with new conditions based on its data table information</t>
   </si>
 </sst>
 </file>
@@ -377,9 +488,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +592,7 @@
       <font>
         <i val="0"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -536,7 +647,7 @@
       <font>
         <i val="0"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -679,17 +790,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB7C8FB5-4A60-4589-8AF2-3974B4223A79}" name="Table2" displayName="Table2" ref="A2:H19" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
-  <autoFilter ref="A2:H19" xr:uid="{FB7C8FB5-4A60-4589-8AF2-3974B4223A79}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB7C8FB5-4A60-4589-8AF2-3974B4223A79}" name="Table2" displayName="Table2" ref="A2:H36" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+  <autoFilter ref="A2:H36" xr:uid="{FB7C8FB5-4A60-4589-8AF2-3974B4223A79}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D94DCF1D-6FD5-453C-A46D-9869C38352C8}" name="Test Number" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{A020788D-1D41-4852-9F55-934D91AFA649}" name="Climate + Season" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{6185D29F-D1FE-4971-966C-56AC01B5DC76}" name="Test" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{CC5DF699-CAB0-42B7-9B93-2010CA39B689}" name="Expected Behaviour" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{2376F1A1-CD88-4A07-B52B-FC693313EC8D}" name="Actual Behaviour" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{2376F1A1-CD88-4A07-B52B-FC693313EC8D}" name="Actual Behaviour" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{BD349D04-C2F0-46B6-B369-DBCD3900AEDA}" name="Time" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{8DAE1A83-CC84-487F-BD95-98F6B547DCD1}" name="Success?" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{8BF98F09-E2CC-4F11-8A7A-A33C92D265B4}" name="Fix" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{8DAE1A83-CC84-487F-BD95-98F6B547DCD1}" name="Success?" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{8BF98F09-E2CC-4F11-8A7A-A33C92D265B4}" name="Fix" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1012,22 +1123,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4EA2CC5-2E47-478A-8876-EC323C3D42FE}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="94.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="120.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="76.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1065,7 +1176,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1090,7 +1201,9 @@
       <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="11"/>
+      <c r="H3" s="11" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -1100,19 +1213,19 @@
         <v>12</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="10">
         <v>45702.578472222223</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="6"/>
     </row>
@@ -1127,16 +1240,16 @@
         <v>14</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="F5" s="10">
         <v>45702.595138888886</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="6"/>
     </row>
@@ -1145,22 +1258,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="F6" s="10">
         <v>45702.598611111112</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -1169,16 +1282,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="F7" s="10">
         <v>45702.606944444444</v>
@@ -1187,7 +1300,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1195,22 +1308,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="10">
         <v>45702.607638888891</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="6"/>
     </row>
@@ -1225,10 +1338,10 @@
         <v>14</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>32</v>
       </c>
       <c r="F9" s="10">
         <v>45702.619444444441</v>
@@ -1237,30 +1350,30 @@
         <v>9</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="8">
         <v>45702.626388888886</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>19</v>
+      <c r="G10" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="H10" s="6"/>
     </row>
@@ -1278,16 +1391,16 @@
         <v>7</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="10">
         <v>45702.629166666666</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1304,7 +1417,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="10">
         <v>45702.632638888892</v>
@@ -1313,168 +1426,626 @@
         <v>9</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="10">
+        <v>45702.720138888886</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="18">
-        <v>45702.720138888886</v>
-      </c>
-      <c r="G13" s="17" t="s">
+      <c r="D14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="10">
+        <v>45702.743055555555</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="10">
+        <v>45702.744444444441</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="10">
+        <v>45702.745833333334</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="10">
+        <v>45702.75</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>16</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="17">
+        <v>45703.786805555559</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>17</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="10">
+        <v>45703.522222222222</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>18</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="10">
+        <v>45703.529861111114</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <v>19</v>
       </c>
-      <c r="H13" s="17"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17" t="s">
+      <c r="B21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="10">
+        <v>45703.541666666664</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>20</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="17">
+        <v>45703.550694444442</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>21</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="17">
+        <v>45703.574999999997</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="17">
+        <v>45703.581250000003</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>23</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="17">
+        <v>45703.585416666669</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>24</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="17">
+        <v>45703.594444444447</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
         <v>25</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="18">
-        <v>45702.743055555555</v>
-      </c>
-      <c r="G14" s="17" t="s">
+      <c r="B27" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="17">
+        <v>45703.642361111109</v>
+      </c>
+      <c r="G27" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="18">
-        <v>45702.744444444441</v>
-      </c>
-      <c r="G15" s="17" t="s">
+      <c r="H27" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>26</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="17">
+        <v>45703.609027777777</v>
+      </c>
+      <c r="G28" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="18">
-        <v>45702.745833333334</v>
-      </c>
-      <c r="G16" s="17" t="s">
+      <c r="H28" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>27</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="17">
+        <v>45703.618750000001</v>
+      </c>
+      <c r="G29" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="18">
-        <v>45702.75</v>
-      </c>
-      <c r="G17" s="17" t="s">
+      <c r="H29" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>28</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="17">
+        <v>45703.636805555558</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>29</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="17">
+        <v>45703.647222222222</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>30</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="17">
+        <v>45703.65347222222</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="16"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>31</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="17">
+        <v>45703.655555555553</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>32</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="18">
-        <v>45703.786805555559</v>
-      </c>
-      <c r="G18" s="17" t="s">
+      <c r="C34" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="17">
+        <v>45703.701388888891</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" s="16"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>33</v>
+      </c>
+      <c r="B35" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="C35" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" s="17">
+        <v>45703.70208333333</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="16"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>34</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="17">
+        <v>45703.702777777777</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G3:G362">
+  <conditionalFormatting sqref="G3:G375">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Indeterminate">
       <formula>NOT(ISERROR(SEARCH("Indeterminate",G3)))</formula>
     </cfRule>

</xml_diff>